<commit_message>
Updated data dictionary and data model flowchart with new data types and configurations
</commit_message>
<xml_diff>
--- a/doc/data_dictionary.xlsx
+++ b/doc/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\LittleLemon\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91F2F1E-2B74-415A-B1FC-73AABECCB184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622EF5EB-0777-4A5F-8127-78C02465AEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D7D26F7-E0F6-4F7E-8AAB-DA80972C7B56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{2D7D26F7-E0F6-4F7E-8AAB-DA80972C7B56}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
   <si>
     <t>Column Name</t>
   </si>
@@ -67,9 +67,6 @@
     <t>uint</t>
   </si>
   <si>
-    <t>char(255)</t>
-  </si>
-  <si>
     <t>Starter</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>date_added</t>
-  </si>
-  <si>
     <t>featured</t>
   </si>
   <si>
@@ -115,12 +109,6 @@
     <t>decimal</t>
   </si>
   <si>
-    <t>char(510)</t>
-  </si>
-  <si>
-    <t>char(1020)</t>
-  </si>
-  <si>
     <t>char(32)</t>
   </si>
   <si>
@@ -290,6 +278,18 @@
   </si>
   <si>
     <t>The qunatity of the menu item.</t>
+  </si>
+  <si>
+    <t>char(64)</t>
+  </si>
+  <si>
+    <t>char(320)</t>
+  </si>
+  <si>
+    <t>char(640)</t>
+  </si>
+  <si>
+    <t>created_date_time</t>
   </si>
 </sst>
 </file>
@@ -342,10 +342,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42E7E8A-188D-429E-B782-DBF1ECFB1A7F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -736,16 +736,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -759,12 +759,12 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
@@ -790,7 +790,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -807,36 +807,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -858,50 +858,50 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E8" s="3">
         <v>10</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -918,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3">
         <v>12</v>
@@ -926,33 +926,33 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="4">
-        <v>45633</v>
+        <v>35</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>1</v>
@@ -968,7 +968,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,7 +999,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1008,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -1016,33 +1016,33 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="3">
         <v>861234567</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -1067,36 +1067,36 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1157,24 +1157,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1183,7 +1183,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1200,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1208,16 +1208,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E6">
         <v>12.5</v>
@@ -1225,16 +1225,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1324,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1332,16 +1332,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5">
         <v>12.5</v>
@@ -1356,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC445FB7-8610-43B3-9ABC-9B45DEC88A7F}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -1405,67 +1405,67 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E6" s="3">
         <v>12.5</v>
@@ -1473,19 +1473,19 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>